<commit_message>
1er grosse partie du tableau jury
</commit_message>
<xml_diff>
--- a/data/example.xlsx
+++ b/data/example.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
   <si>
     <t>codenip</t>
   </si>
@@ -29,49 +29,70 @@
     <t>parcours</t>
   </si>
   <si>
-    <t>NETU8918 Pe.</t>
-  </si>
-  <si>
-    <t>Petu8918</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>NETU8811 Pe.</t>
-  </si>
-  <si>
-    <t>Petu8811</t>
-  </si>
-  <si>
-    <t>NETU8884 Pe.</t>
-  </si>
-  <si>
-    <t>Petu8884</t>
-  </si>
-  <si>
-    <t>NETU8874 Pe.</t>
-  </si>
-  <si>
-    <t>Petu8874</t>
-  </si>
-  <si>
-    <t>NETU8888 Pe.</t>
-  </si>
-  <si>
-    <t>Petu8888</t>
-  </si>
-  <si>
-    <t>NETU8834 Pe.</t>
-  </si>
-  <si>
-    <t>Petu8834</t>
-  </si>
-  <si>
-    <t>NETU8840 Pe.</t>
-  </si>
-  <si>
-    <t>Petu8840</t>
+    <t>Etudiant 1</t>
+  </si>
+  <si>
+    <t>Prenom1</t>
+  </si>
+  <si>
+    <t>Parcours 1</t>
+  </si>
+  <si>
+    <t>Etudiant 2</t>
+  </si>
+  <si>
+    <t>Prenom2</t>
+  </si>
+  <si>
+    <t>Parcours 2</t>
+  </si>
+  <si>
+    <t>Etudiant 3</t>
+  </si>
+  <si>
+    <t>Prenom3</t>
+  </si>
+  <si>
+    <t>Parcours 3</t>
+  </si>
+  <si>
+    <t>Etudiant 4</t>
+  </si>
+  <si>
+    <t>Prenom4</t>
+  </si>
+  <si>
+    <t>Parcours 4</t>
+  </si>
+  <si>
+    <t>Etudiant 5</t>
+  </si>
+  <si>
+    <t>Prenom5</t>
+  </si>
+  <si>
+    <t>Parcours 5</t>
+  </si>
+  <si>
+    <t>Compétence 1</t>
+  </si>
+  <si>
+    <t>Compétence 2</t>
+  </si>
+  <si>
+    <t>Compétence 3</t>
+  </si>
+  <si>
+    <t>Compétence 4</t>
+  </si>
+  <si>
+    <t>Compétence 5</t>
+  </si>
+  <si>
+    <t>ADM</t>
+  </si>
+  <si>
+    <t>NAR</t>
   </si>
 </sst>
 </file>
@@ -411,7 +432,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:Q6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -419,23 +440,38 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
+    <row r="1" spans="1:17">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:17">
       <c r="A2">
-        <v>8918</v>
+        <v>12345</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -446,10 +482,16 @@
       <c r="D2" t="s">
         <v>6</v>
       </c>
+      <c r="G2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:17">
       <c r="A3">
-        <v>8811</v>
+        <v>67890</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -458,77 +500,55 @@
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>9</v>
+      </c>
+      <c r="G3" t="s">
+        <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:17">
       <c r="A4">
-        <v>8884</v>
+        <v>54321</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:17">
       <c r="A5">
-        <v>8874</v>
+        <v>98765</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:17">
       <c r="A6">
-        <v>8888</v>
+        <v>13579</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7">
-        <v>8834</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8">
-        <v>8840</v>
-      </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" t="s">
         <v>18</v>
-      </c>
-      <c r="D8" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>